<commit_message>
3.2.8 LKey process delete
</commit_message>
<xml_diff>
--- a/voqui/bin/Debug/VOQ3D0.xlsx
+++ b/voqui/bin/Debug/VOQ3D0.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="13860" windowHeight="8550" tabRatio="667" activeTab="3"/>
+    <workbookView xWindow="3228" yWindow="2400" windowWidth="14376" windowHeight="8904" tabRatio="667" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="journal" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="79">
   <si>
     <t xml:space="preserve">ｺｰﾄﾞ</t>
   </si>
@@ -250,7 +250,7 @@
     <t xml:space="preserve">FGK-SYSTEMS 2020</t>
   </si>
   <si>
-    <t xml:space="preserve">(2020/1/1-2020/12/31)</t>
+    <t xml:space="preserve">(2020/1/1-2020/12/31) aa</t>
   </si>
   <si>
     <t xml:space="preserve">01/01 1001</t>
@@ -304,19 +304,40 @@
     <t xml:space="preserve">事業主貸</t>
   </si>
   <si>
+    <t xml:space="preserve">事業費調整</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/20 1006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">入金（善光）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/31 1007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">旅費交通費</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/04 1008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">接待交際費</t>
+  </si>
+  <si>
     <t xml:space="preserve">現金　　</t>
   </si>
   <si>
-    <t xml:space="preserve">事業費調整</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01/20 1006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">売掛金　</t>
-  </si>
-  <si>
-    <t xml:space="preserve">入金（善光）</t>
+    <t xml:space="preserve">aaa33445566</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
@@ -1206,20 +1227,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="3.125" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="77" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="77" customWidth="1"/>
     <col min="3" max="3" width="6" style="81" customWidth="1"/>
-    <col min="4" max="4" width="11.625" style="81" customWidth="1"/>
-    <col min="5" max="5" width="6.125" style="81" customWidth="1"/>
-    <col min="6" max="6" width="11.75" style="81" customWidth="1"/>
-    <col min="7" max="7" width="12.75" style="89" customWidth="1"/>
-    <col min="8" max="8" width="30.625" style="82" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="81" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" style="81" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="81" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="89" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" style="82" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18.75" customHeight="1">
@@ -1297,7 +1316,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:22" s="11" customFormat="1" ht="14.25" thickTop="1">
+    <row r="5" spans="1:22" s="11" customFormat="1" ht="13.8" thickTop="1">
       <c r="A5" s="9"/>
       <c r="B5" s="77"/>
       <c r="C5" s="81"/>
@@ -1404,36 +1423,82 @@
         <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="G9" s="92">
         <v>1337899</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
         <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G10" s="92">
         <v>220000</v>
       </c>
       <c r="H10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
         <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="92">
+        <v>1500</v>
+      </c>
+      <c r="H11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="92">
+        <v>5566</v>
+      </c>
+      <c r="H12" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1456,26 +1521,26 @@
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="4.625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="13.125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="13" customWidth="1"/>
     <col min="5" max="5" width="5" style="14" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="15" customWidth="1"/>
-    <col min="7" max="7" width="31.25" style="15" customWidth="1"/>
-    <col min="8" max="9" width="9.875" style="16" customWidth="1"/>
-    <col min="10" max="10" width="3.25" style="17" customWidth="1"/>
-    <col min="11" max="11" width="9.875" style="16" customWidth="1"/>
-    <col min="12" max="12" width="11.125" style="16" customWidth="1"/>
-    <col min="13" max="13" width="3.625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="31.21875" style="15" customWidth="1"/>
+    <col min="8" max="9" width="12.77734375" style="16" customWidth="1"/>
+    <col min="10" max="10" width="3.21875" style="17" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" style="16" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="16" customWidth="1"/>
+    <col min="13" max="13" width="3.6640625" style="16" customWidth="1"/>
     <col min="14" max="17" width="10" style="16" customWidth="1"/>
     <col min="18" max="18" width="4" style="18" customWidth="1"/>
-    <col min="19" max="19" width="5.375" style="13" customWidth="1"/>
+    <col min="19" max="19" width="5.33203125" style="13" customWidth="1"/>
     <col min="20" max="20" width="22" style="13" customWidth="1"/>
     <col min="21" max="16384" width="9" style="13"/>
   </cols>
@@ -1533,7 +1598,7 @@
       <c r="S4" s="22"/>
       <c r="T4" s="22"/>
     </row>
-    <row r="5" spans="2:20" ht="14.25" thickTop="1">
+    <row r="5" spans="2:20" ht="13.8" thickTop="1">
       <c r="B5" s="29"/>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -1571,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="K6" s="92">
         <v>2337899</v>
@@ -1590,7 +1655,7 @@
         <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" s="92">
         <v>0</v>
@@ -1599,7 +1664,7 @@
         <v>1337899</v>
       </c>
       <c r="J7" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="K7" s="92">
         <v>1000000</v>
@@ -1609,16 +1674,16 @@
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
         <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H8" s="92">
         <v>220000</v>
@@ -1627,292 +1692,426 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="K8" s="92">
         <v>1220000</v>
       </c>
     </row>
-    <row r="9"/>
+    <row r="9">
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="92">
+        <v>0</v>
+      </c>
+      <c r="I9" s="92">
+        <v>1500</v>
+      </c>
+      <c r="J9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="92">
+        <v>1218500</v>
+      </c>
+    </row>
     <row r="10">
-      <c r="B10" s="91"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="91"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="91"/>
-    </row>
-    <row r="11">
-      <c r="B11" t="s">
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="92">
+        <v>0</v>
+      </c>
+      <c r="I10" s="92">
+        <v>5566</v>
+      </c>
+      <c r="J10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="92">
+        <v>1212934</v>
+      </c>
+    </row>
+    <row r="11"/>
+    <row r="12">
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="91"/>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" t="s">
         <v>44</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E13" t="s">
         <v>41</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F13" t="s">
         <v>42</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G13" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="92">
+      <c r="H13" s="92">
         <v>400000</v>
       </c>
-      <c r="I11" s="92">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="I13" s="92">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="92">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="92">
+        <v>0</v>
+      </c>
+      <c r="I14" s="92">
+        <v>220000</v>
+      </c>
+      <c r="J14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="92">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="15"/>
+    <row r="16">
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="91"/>
+      <c r="G16" s="91"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="91"/>
+      <c r="J16" s="91"/>
+      <c r="K16" s="91"/>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="92">
+        <v>151200</v>
+      </c>
+      <c r="I17" s="92">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" s="92">
+        <v>151200</v>
+      </c>
+    </row>
+    <row r="18"/>
+    <row r="19">
+      <c r="B19" s="91"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="91"/>
+      <c r="H19" s="91"/>
+      <c r="I19" s="91"/>
+      <c r="J19" s="91"/>
+      <c r="K19" s="91"/>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="92">
+        <v>1337899</v>
+      </c>
+      <c r="I20" s="92">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" s="92">
+        <v>1337899</v>
+      </c>
+    </row>
+    <row r="21"/>
+    <row r="22">
+      <c r="B22" s="91"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="91"/>
+      <c r="I22" s="91"/>
+      <c r="J22" s="91"/>
+      <c r="K22" s="91"/>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="92">
+        <v>0</v>
+      </c>
+      <c r="I23" s="92">
+        <v>2337899</v>
+      </c>
+      <c r="J23" t="s">
+        <v>68</v>
+      </c>
+      <c r="K23" s="92">
+        <v>2337899</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="92">
+        <v>0</v>
+      </c>
+      <c r="I24" s="92">
+        <v>400000</v>
+      </c>
+      <c r="J24" t="s">
+        <v>68</v>
+      </c>
+      <c r="K24" s="92">
+        <v>2737899</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="92">
+        <v>0</v>
+      </c>
+      <c r="I25" s="92">
+        <v>151200</v>
+      </c>
+      <c r="J25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" s="92">
+        <v>2889099</v>
+      </c>
+    </row>
+    <row r="26"/>
+    <row r="27">
+      <c r="B27" s="91"/>
+      <c r="C27" s="91"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="91"/>
+      <c r="G27" s="91"/>
+      <c r="H27" s="91"/>
+      <c r="I27" s="91"/>
+      <c r="J27" s="91"/>
+      <c r="K27" s="91"/>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="92">
+        <v>5566</v>
+      </c>
+      <c r="I28" s="92">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>67</v>
+      </c>
+      <c r="K28" s="92">
+        <v>5566</v>
+      </c>
+    </row>
+    <row r="29"/>
+    <row r="30">
+      <c r="B30" s="91"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="91"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="91"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="91"/>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="92">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" t="s">
         <v>39</v>
       </c>
-      <c r="F12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="92">
-        <v>0</v>
-      </c>
-      <c r="I12" s="92">
-        <v>220000</v>
-      </c>
-      <c r="J12" t="s">
-        <v>60</v>
-      </c>
-      <c r="K12" s="92">
-        <v>180000</v>
-      </c>
-    </row>
-    <row r="13"/>
-    <row r="14">
-      <c r="B14" s="91"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="91"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="91"/>
-    </row>
-    <row r="15">
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="92">
-        <v>151200</v>
-      </c>
-      <c r="I15" s="92">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>60</v>
-      </c>
-      <c r="K15" s="92">
-        <v>151200</v>
-      </c>
-    </row>
-    <row r="16"/>
-    <row r="17">
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="91"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="91"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="91"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="91"/>
-      <c r="K17" s="91"/>
-    </row>
-    <row r="18">
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="92">
-        <v>1337899</v>
-      </c>
-      <c r="I18" s="92">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>60</v>
-      </c>
-      <c r="K18" s="92">
-        <v>1337899</v>
-      </c>
-    </row>
-    <row r="19"/>
-    <row r="20">
-      <c r="B20" s="91"/>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="91"/>
-      <c r="K20" s="91"/>
-    </row>
-    <row r="21">
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="F31" t="s">
         <v>40</v>
       </c>
-      <c r="G21" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="92">
-        <v>0</v>
-      </c>
-      <c r="I21" s="92">
-        <v>2337899</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="G31" t="s">
         <v>61</v>
       </c>
-      <c r="K21" s="92">
-        <v>2337899</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="92">
-        <v>0</v>
-      </c>
-      <c r="I22" s="92">
-        <v>400000</v>
-      </c>
-      <c r="J22" t="s">
-        <v>61</v>
-      </c>
-      <c r="K22" s="92">
-        <v>2737899</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" t="s">
-        <v>51</v>
-      </c>
-      <c r="H23" s="92">
-        <v>0</v>
-      </c>
-      <c r="I23" s="92">
-        <v>151200</v>
-      </c>
-      <c r="J23" t="s">
-        <v>61</v>
-      </c>
-      <c r="K23" s="92">
-        <v>2889099</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11">
-      <c r="B24" s="63"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="20"/>
+      <c r="H31" s="92">
+        <v>1500</v>
+      </c>
+      <c r="I31" s="92">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>67</v>
+      </c>
+      <c r="K31" s="92">
+        <v>1500</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="fullwidthKatakana"/>
   <pageMargins left="1.10236220472441" right="0.708661417322835" top="0.748031496062992" bottom="0.748031496062992" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" horizontalDpi="-3" verticalDpi="-3" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="portrait" horizontalDpi="-3" verticalDpi="-3" r:id="rId1"/>
   <headerFooter>
     <oddFooter><![CDATA[&C(&P/&N)]]></oddFooter>
   </headerFooter>
@@ -1926,17 +2125,16 @@
   </sheetPr>
   <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="2.25" style="13" customWidth="1"/>
-    <col min="2" max="3" width="10.75" style="16" customWidth="1"/>
+    <col min="1" max="1" width="2.21875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="16" customWidth="1"/>
     <col min="4" max="4" width="13" style="36" customWidth="1"/>
-    <col min="5" max="5" width="23.375" style="35" customWidth="1"/>
-    <col min="6" max="7" width="10.75" style="16" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="35" customWidth="1"/>
+    <col min="6" max="7" width="12.77734375" style="16" customWidth="1"/>
     <col min="8" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
@@ -1978,10 +2176,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="14.25" thickTop="1"/>
+    <row r="5" spans="2:7" ht="13.8" thickTop="1"/>
     <row r="6">
       <c r="B6" s="92">
-        <v>1220000</v>
+        <v>1212934</v>
       </c>
       <c r="C6" s="92">
         <v>2557899</v>
@@ -1993,7 +2191,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="92">
-        <v>1337899</v>
+        <v>1344965</v>
       </c>
       <c r="G6" s="92">
         <v>0</v>
@@ -2061,7 +2259,7 @@
     </row>
     <row r="10">
       <c r="B10" s="93">
-        <v>2889099</v>
+        <v>2882033</v>
       </c>
       <c r="C10" s="93">
         <v>4446998</v>
@@ -2071,7 +2269,7 @@
       </c>
       <c r="E10" s="93"/>
       <c r="F10" s="93">
-        <v>1557899</v>
+        <v>1564965</v>
       </c>
       <c r="G10" s="93">
         <v>0</v>
@@ -2118,54 +2316,81 @@
     </row>
     <row r="14"/>
     <row r="15">
-      <c r="B15" s="93">
+      <c r="B15" s="92">
+        <v>5566</v>
+      </c>
+      <c r="C15" s="92">
+        <v>5566</v>
+      </c>
+      <c r="D15" s="92">
+        <v>515</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="92">
+        <v>0</v>
+      </c>
+      <c r="G15" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="92">
+        <v>1500</v>
+      </c>
+      <c r="C16" s="92">
+        <v>1500</v>
+      </c>
+      <c r="D16" s="92">
+        <v>517</v>
+      </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="92">
+        <v>0</v>
+      </c>
+      <c r="G16" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="93">
+        <v>7066</v>
+      </c>
+      <c r="C17" s="93">
+        <v>7066</v>
+      </c>
+      <c r="D17" s="93">
+        <v>500</v>
+      </c>
+      <c r="E17" s="93"/>
+      <c r="F17" s="93">
+        <v>0</v>
+      </c>
+      <c r="G17" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18"/>
+    <row r="19">
+      <c r="B19" s="93">
         <v>2889099</v>
       </c>
-      <c r="C15" s="93">
-        <v>4446998</v>
-      </c>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93">
-        <v>4446998</v>
-      </c>
-      <c r="G15" s="93">
+      <c r="C19" s="93">
+        <v>4454064</v>
+      </c>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="93">
+        <v>4454064</v>
+      </c>
+      <c r="G19" s="93">
         <v>2889099</v>
       </c>
     </row>
-    <row r="16"/>
-    <row r="17" spans="2:7">
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-    </row>
+    <row r="20"/>
     <row r="21" spans="2:7">
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
@@ -2189,20 +2414,18 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="1.5" style="13" customWidth="1"/>
-    <col min="2" max="2" width="3.25" style="13" customWidth="1"/>
+    <col min="1" max="1" width="1.44140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="3.21875" style="13" customWidth="1"/>
     <col min="3" max="3" width="25" style="13" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="98" customWidth="1"/>
-    <col min="5" max="5" width="4.875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="3.25" style="13" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="98" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="3.21875" style="13" customWidth="1"/>
     <col min="7" max="7" width="25" style="13" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="102" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="102" customWidth="1"/>
     <col min="9" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
@@ -2233,7 +2456,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
@@ -2247,12 +2470,12 @@
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C7"/>
       <c r="D7" s="92"/>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G7"/>
       <c r="H7" s="92"/>
@@ -2263,7 +2486,7 @@
         <v>40</v>
       </c>
       <c r="D8" s="92">
-        <v>1220000</v>
+        <v>1212934</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
@@ -2292,7 +2515,7 @@
         <v>151200</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="G10"/>
       <c r="H10" s="92"/>
@@ -2319,17 +2542,17 @@
       <c r="D12"/>
       <c r="F12"/>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="H12" s="92">
-        <v>0</v>
+        <v>-7066</v>
       </c>
     </row>
     <row r="13">
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13" s="93">
-        <v>2889099</v>
+        <v>2882033</v>
       </c>
     </row>
     <row r="14">
@@ -2341,13 +2564,13 @@
       <c r="B15" s="93"/>
       <c r="C15" s="93"/>
       <c r="D15" s="93">
-        <v>2889099</v>
+        <v>2882033</v>
       </c>
       <c r="E15" s="93"/>
       <c r="F15" s="93"/>
       <c r="G15" s="93"/>
       <c r="H15" s="93">
-        <v>2889099</v>
+        <v>2882033</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2361,7 +2584,7 @@
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18">
@@ -2375,21 +2598,23 @@
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C19"/>
       <c r="D19" s="92"/>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G19"/>
       <c r="H19" s="92"/>
     </row>
     <row r="20">
       <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20" s="93">
-        <v>0</v>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="92">
+        <v>5566</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -2397,60 +2622,73 @@
     </row>
     <row r="21">
       <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21" s="92"/>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="92">
+        <v>1500</v>
+      </c>
       <c r="F21"/>
       <c r="G21"/>
       <c r="H21"/>
     </row>
     <row r="22">
-      <c r="B22" t="s">
-        <v>71</v>
-      </c>
+      <c r="B22"/>
       <c r="C22"/>
-      <c r="D22" s="92"/>
+      <c r="D22" s="93">
+        <v>7066</v>
+      </c>
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
     </row>
     <row r="23">
       <c r="B23"/>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="92">
-        <v>0</v>
-      </c>
+      <c r="C23"/>
+      <c r="D23" s="92"/>
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
     </row>
     <row r="24">
-      <c r="B24"/>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
       <c r="C24"/>
-      <c r="D24"/>
+      <c r="D24" s="92"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
     </row>
     <row r="25">
-      <c r="B25" s="93"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93">
-        <v>0</v>
-      </c>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="99"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="103"/>
+      <c r="B25"/>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="92">
+        <v>-7066</v>
+      </c>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+    </row>
+    <row r="26">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="93"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93">
+        <v>0</v>
+      </c>
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="93">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="fullwidthKatakana"/>

</xml_diff>

<commit_message>
sub window2 update b
</commit_message>
<xml_diff>
--- a/voqui/bin/Debug/VOQ3D0.xlsx
+++ b/voqui/bin/Debug/VOQ3D0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="82">
   <si>
     <t xml:space="preserve">ｺｰﾄﾞ</t>
   </si>
@@ -334,10 +334,19 @@
     <t xml:space="preserve">接待交際費</t>
   </si>
   <si>
-    <t xml:space="preserve">現金　　</t>
-  </si>
-  <si>
     <t xml:space="preserve">aaa33445566</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/05 1009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">荷造運賃</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hhhuuu</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
@@ -1492,13 +1501,36 @@
         <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="G12" s="92">
         <v>5566</v>
       </c>
       <c r="H12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
         <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="92">
+        <v>8888</v>
+      </c>
+      <c r="H13" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1636,7 +1668,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K6" s="92">
         <v>2337899</v>
@@ -1664,7 +1696,7 @@
         <v>1337899</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K7" s="92">
         <v>1000000</v>
@@ -1692,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K8" s="92">
         <v>1220000</v>
@@ -1720,7 +1752,7 @@
         <v>1500</v>
       </c>
       <c r="J9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K9" s="92">
         <v>1218500</v>
@@ -1739,7 +1771,7 @@
         <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H10" s="92">
         <v>0</v>
@@ -1748,363 +1780,436 @@
         <v>5566</v>
       </c>
       <c r="J10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K10" s="92">
         <v>1212934</v>
       </c>
     </row>
-    <row r="11"/>
-    <row r="12">
-      <c r="B12" s="91"/>
-      <c r="C12" s="91"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="91"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="91"/>
-      <c r="I12" s="91"/>
-      <c r="J12" s="91"/>
-      <c r="K12" s="91"/>
-    </row>
+    <row r="11">
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="92">
+        <v>0</v>
+      </c>
+      <c r="I11" s="92">
+        <v>8888</v>
+      </c>
+      <c r="J11" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="92">
+        <v>1204046</v>
+      </c>
+    </row>
+    <row r="12"/>
     <row r="13">
-      <c r="B13" t="s">
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>44</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>41</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>42</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="92">
+      <c r="H14" s="92">
         <v>400000</v>
       </c>
-      <c r="I13" s="92">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>67</v>
-      </c>
-      <c r="K13" s="92">
+      <c r="I14" s="92">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14" s="92">
         <v>400000</v>
       </c>
     </row>
-    <row r="14">
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14" t="s">
+    <row r="15">
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15" t="s">
         <v>56</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>39</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>40</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="92">
-        <v>0</v>
-      </c>
-      <c r="I14" s="92">
+      <c r="H15" s="92">
+        <v>0</v>
+      </c>
+      <c r="I15" s="92">
         <v>220000</v>
       </c>
-      <c r="J14" t="s">
-        <v>67</v>
-      </c>
-      <c r="K14" s="92">
+      <c r="J15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="92">
         <v>180000</v>
       </c>
     </row>
-    <row r="15"/>
-    <row r="16">
-      <c r="B16" s="91"/>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="91"/>
-      <c r="K16" s="91"/>
-    </row>
+    <row r="16"/>
     <row r="17">
-      <c r="B17" t="s">
+      <c r="B17" s="91"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="91"/>
+      <c r="G17" s="91"/>
+      <c r="H17" s="91"/>
+      <c r="I17" s="91"/>
+      <c r="J17" s="91"/>
+      <c r="K17" s="91"/>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
         <v>49</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>48</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>41</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>42</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G18" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="92">
+      <c r="H18" s="92">
         <v>151200</v>
       </c>
-      <c r="I17" s="92">
-        <v>0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>67</v>
-      </c>
-      <c r="K17" s="92">
+      <c r="I18" s="92">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>70</v>
+      </c>
+      <c r="K18" s="92">
         <v>151200</v>
       </c>
     </row>
-    <row r="18"/>
-    <row r="19">
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="91"/>
-      <c r="H19" s="91"/>
-      <c r="I19" s="91"/>
-      <c r="J19" s="91"/>
-      <c r="K19" s="91"/>
-    </row>
+    <row r="19"/>
     <row r="20">
-      <c r="B20" t="s">
+      <c r="B20" s="91"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
+      <c r="G20" s="91"/>
+      <c r="H20" s="91"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="91"/>
+      <c r="K20" s="91"/>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>54</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>52</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>39</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>40</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>55</v>
       </c>
-      <c r="H20" s="92">
+      <c r="H21" s="92">
         <v>1337899</v>
       </c>
-      <c r="I20" s="92">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>67</v>
-      </c>
-      <c r="K20" s="92">
+      <c r="I21" s="92">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" s="92">
         <v>1337899</v>
       </c>
     </row>
-    <row r="21"/>
-    <row r="22">
-      <c r="B22" s="91"/>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="91"/>
-      <c r="I22" s="91"/>
-      <c r="J22" s="91"/>
-      <c r="K22" s="91"/>
-    </row>
+    <row r="22"/>
     <row r="23">
-      <c r="B23" t="s">
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="91"/>
+      <c r="H23" s="91"/>
+      <c r="I23" s="91"/>
+      <c r="J23" s="91"/>
+      <c r="K23" s="91"/>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>42</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>38</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>39</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>40</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="92">
-        <v>0</v>
-      </c>
-      <c r="I23" s="92">
+      <c r="H24" s="92">
+        <v>0</v>
+      </c>
+      <c r="I24" s="92">
         <v>2337899</v>
       </c>
-      <c r="J23" t="s">
-        <v>68</v>
-      </c>
-      <c r="K23" s="92">
+      <c r="J24" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24" s="92">
         <v>2337899</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" t="s">
-        <v>47</v>
-      </c>
-      <c r="H24" s="92">
-        <v>0</v>
-      </c>
-      <c r="I24" s="92">
-        <v>400000</v>
-      </c>
-      <c r="J24" t="s">
-        <v>68</v>
-      </c>
-      <c r="K24" s="92">
-        <v>2737899</v>
       </c>
     </row>
     <row r="25">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="92">
+        <v>0</v>
+      </c>
+      <c r="I25" s="92">
+        <v>400000</v>
+      </c>
+      <c r="J25" t="s">
+        <v>71</v>
+      </c>
+      <c r="K25" s="92">
+        <v>2737899</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26" t="s">
         <v>48</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>49</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>50</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G26" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="92">
-        <v>0</v>
-      </c>
-      <c r="I25" s="92">
+      <c r="H26" s="92">
+        <v>0</v>
+      </c>
+      <c r="I26" s="92">
         <v>151200</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J26" t="s">
+        <v>71</v>
+      </c>
+      <c r="K26" s="92">
+        <v>2889099</v>
+      </c>
+    </row>
+    <row r="27"/>
+    <row r="28">
+      <c r="B28" s="91"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="91"/>
+      <c r="H28" s="91"/>
+      <c r="I28" s="91"/>
+      <c r="J28" s="91"/>
+      <c r="K28" s="91"/>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
         <v>68</v>
       </c>
-      <c r="K25" s="92">
-        <v>2889099</v>
-      </c>
-    </row>
-    <row r="26"/>
-    <row r="27">
-      <c r="B27" s="91"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="91"/>
-      <c r="G27" s="91"/>
-      <c r="H27" s="91"/>
-      <c r="I27" s="91"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="91"/>
-    </row>
-    <row r="28">
-      <c r="B28" t="s">
+      <c r="D29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" s="92">
+        <v>8888</v>
+      </c>
+      <c r="I29" s="92">
+        <v>0</v>
+      </c>
+      <c r="J29" t="s">
+        <v>70</v>
+      </c>
+      <c r="K29" s="92">
+        <v>8888</v>
+      </c>
+    </row>
+    <row r="30"/>
+    <row r="31">
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="91"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="91"/>
+      <c r="H31" s="91"/>
+      <c r="I31" s="91"/>
+      <c r="J31" s="91"/>
+      <c r="K31" s="91"/>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
         <v>63</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C32" t="s">
         <v>64</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D32" t="s">
         <v>62</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E32" t="s">
         <v>39</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32" t="s">
         <v>65</v>
       </c>
-      <c r="G28" t="s">
-        <v>66</v>
-      </c>
-      <c r="H28" s="92">
+      <c r="H32" s="92">
         <v>5566</v>
       </c>
-      <c r="I28" s="92">
-        <v>0</v>
-      </c>
-      <c r="J28" t="s">
-        <v>67</v>
-      </c>
-      <c r="K28" s="92">
+      <c r="I32" s="92">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>70</v>
+      </c>
+      <c r="K32" s="92">
         <v>5566</v>
       </c>
     </row>
-    <row r="29"/>
-    <row r="30">
-      <c r="B30" s="91"/>
-      <c r="C30" s="91"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="91"/>
-      <c r="F30" s="91"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="91"/>
-      <c r="I30" s="91"/>
-      <c r="J30" s="91"/>
-      <c r="K30" s="91"/>
-    </row>
-    <row r="31">
-      <c r="B31" t="s">
+    <row r="33"/>
+    <row r="34">
+      <c r="B34" s="91"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="91"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="91"/>
+      <c r="G34" s="91"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="91"/>
+      <c r="J34" s="91"/>
+      <c r="K34" s="91"/>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
         <v>59</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C35" t="s">
         <v>60</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D35" t="s">
         <v>58</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E35" t="s">
         <v>39</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F35" t="s">
         <v>40</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G35" t="s">
         <v>61</v>
       </c>
-      <c r="H31" s="92">
+      <c r="H35" s="92">
         <v>1500</v>
       </c>
-      <c r="I31" s="92">
-        <v>0</v>
-      </c>
-      <c r="J31" t="s">
-        <v>67</v>
-      </c>
-      <c r="K31" s="92">
+      <c r="I35" s="92">
+        <v>0</v>
+      </c>
+      <c r="J35" t="s">
+        <v>70</v>
+      </c>
+      <c r="K35" s="92">
         <v>1500</v>
       </c>
     </row>
@@ -2179,7 +2284,7 @@
     <row r="5" spans="2:7" ht="13.8" thickTop="1"/>
     <row r="6">
       <c r="B6" s="92">
-        <v>1212934</v>
+        <v>1204046</v>
       </c>
       <c r="C6" s="92">
         <v>2557899</v>
@@ -2191,7 +2296,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="92">
-        <v>1344965</v>
+        <v>1353853</v>
       </c>
       <c r="G6" s="92">
         <v>0</v>
@@ -2259,7 +2364,7 @@
     </row>
     <row r="10">
       <c r="B10" s="93">
-        <v>2882033</v>
+        <v>2873145</v>
       </c>
       <c r="C10" s="93">
         <v>4446998</v>
@@ -2269,7 +2374,7 @@
       </c>
       <c r="E10" s="93"/>
       <c r="F10" s="93">
-        <v>1564965</v>
+        <v>1573853</v>
       </c>
       <c r="G10" s="93">
         <v>0</v>
@@ -2317,16 +2422,16 @@
     <row r="14"/>
     <row r="15">
       <c r="B15" s="92">
-        <v>5566</v>
+        <v>8888</v>
       </c>
       <c r="C15" s="92">
-        <v>5566</v>
+        <v>8888</v>
       </c>
       <c r="D15" s="92">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F15" s="92">
         <v>0</v>
@@ -2337,68 +2442,80 @@
     </row>
     <row r="16">
       <c r="B16" s="92">
+        <v>5566</v>
+      </c>
+      <c r="C16" s="92">
+        <v>5566</v>
+      </c>
+      <c r="D16" s="92">
+        <v>515</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="92">
+        <v>0</v>
+      </c>
+      <c r="G16" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="92">
         <v>1500</v>
       </c>
-      <c r="C16" s="92">
+      <c r="C17" s="92">
         <v>1500</v>
       </c>
-      <c r="D16" s="92">
+      <c r="D17" s="92">
         <v>517</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="92">
-        <v>0</v>
-      </c>
-      <c r="G16" s="92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="93">
-        <v>7066</v>
-      </c>
-      <c r="C17" s="93">
-        <v>7066</v>
-      </c>
-      <c r="D17" s="93">
+      <c r="F17" s="92">
+        <v>0</v>
+      </c>
+      <c r="G17" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="93">
+        <v>15954</v>
+      </c>
+      <c r="C18" s="93">
+        <v>15954</v>
+      </c>
+      <c r="D18" s="93">
         <v>500</v>
       </c>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93">
-        <v>0</v>
-      </c>
-      <c r="G17" s="93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18"/>
-    <row r="19">
-      <c r="B19" s="93">
+      <c r="E18" s="93"/>
+      <c r="F18" s="93">
+        <v>0</v>
+      </c>
+      <c r="G18" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19"/>
+    <row r="20">
+      <c r="B20" s="93">
         <v>2889099</v>
       </c>
-      <c r="C19" s="93">
-        <v>4454064</v>
-      </c>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93">
-        <v>4454064</v>
-      </c>
-      <c r="G19" s="93">
+      <c r="C20" s="93">
+        <v>4462952</v>
+      </c>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93">
+        <v>4462952</v>
+      </c>
+      <c r="G20" s="93">
         <v>2889099</v>
       </c>
     </row>
-    <row r="20"/>
-    <row r="21" spans="2:7">
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-    </row>
+    <row r="21"/>
   </sheetData>
   <phoneticPr fontId="1" type="fullwidthKatakana"/>
   <pageMargins left="0.984251968503937" right="0.708661417322835" top="0.748031496062992" bottom="0.748031496062992" header="0.31496062992126" footer="0.31496062992126"/>
@@ -2456,7 +2573,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
@@ -2470,12 +2587,12 @@
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C7"/>
       <c r="D7" s="92"/>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G7"/>
       <c r="H7" s="92"/>
@@ -2486,7 +2603,7 @@
         <v>40</v>
       </c>
       <c r="D8" s="92">
-        <v>1212934</v>
+        <v>1204046</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
@@ -2515,7 +2632,7 @@
         <v>151200</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G10"/>
       <c r="H10" s="92"/>
@@ -2542,17 +2659,17 @@
       <c r="D12"/>
       <c r="F12"/>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H12" s="92">
-        <v>-7066</v>
+        <v>-15954</v>
       </c>
     </row>
     <row r="13">
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13" s="93">
-        <v>2882033</v>
+        <v>2873145</v>
       </c>
     </row>
     <row r="14">
@@ -2564,13 +2681,13 @@
       <c r="B15" s="93"/>
       <c r="C15" s="93"/>
       <c r="D15" s="93">
-        <v>2882033</v>
+        <v>2873145</v>
       </c>
       <c r="E15" s="93"/>
       <c r="F15" s="93"/>
       <c r="G15" s="93"/>
       <c r="H15" s="93">
-        <v>2882033</v>
+        <v>2873145</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2584,7 +2701,7 @@
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
@@ -2598,12 +2715,12 @@
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C19"/>
       <c r="D19" s="92"/>
       <c r="F19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G19"/>
       <c r="H19" s="92"/>
@@ -2611,10 +2728,10 @@
     <row r="20">
       <c r="B20"/>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D20" s="92">
-        <v>5566</v>
+        <v>8888</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -2623,10 +2740,10 @@
     <row r="21">
       <c r="B21"/>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D21" s="92">
-        <v>1500</v>
+        <v>5566</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
@@ -2634,9 +2751,11 @@
     </row>
     <row r="22">
       <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22" s="93">
-        <v>7066</v>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="92">
+        <v>1500</v>
       </c>
       <c r="F22"/>
       <c r="G22"/>
@@ -2645,15 +2764,15 @@
     <row r="23">
       <c r="B23"/>
       <c r="C23"/>
-      <c r="D23" s="92"/>
+      <c r="D23" s="93">
+        <v>15954</v>
+      </c>
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
     </row>
     <row r="24">
-      <c r="B24" t="s">
-        <v>78</v>
-      </c>
+      <c r="B24"/>
       <c r="C24"/>
       <c r="D24" s="92"/>
       <c r="F24"/>
@@ -2661,32 +2780,42 @@
       <c r="H24"/>
     </row>
     <row r="25">
-      <c r="B25"/>
-      <c r="C25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="92">
-        <v>-7066</v>
-      </c>
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25"/>
+      <c r="D25" s="92"/>
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
     </row>
     <row r="26">
       <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="92">
+        <v>-15954</v>
+      </c>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
     </row>
     <row r="27">
-      <c r="B27" s="93"/>
-      <c r="C27" s="93"/>
-      <c r="D27" s="93">
-        <v>0</v>
-      </c>
-      <c r="E27" s="93"/>
-      <c r="F27" s="93"/>
-      <c r="G27" s="93"/>
-      <c r="H27" s="93">
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="93"/>
+      <c r="C28" s="93"/>
+      <c r="D28" s="93">
+        <v>0</v>
+      </c>
+      <c r="E28" s="93"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="93"/>
+      <c r="H28" s="93">
         <v>0</v>
       </c>
     </row>

</xml_diff>